<commit_message>
CIERRE 1 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/ENTRADAS OBRADOR     M A Y O        2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/ENTRADAS OBRADOR     M A Y O        2022.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="467">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1428,6 +1428,21 @@
   </si>
   <si>
     <t>20495--10981</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA EL TOPETE   244</t>
+  </si>
+  <si>
+    <t>CANALES  199-5</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA EL TOPETE   246</t>
+  </si>
+  <si>
+    <t>CANALES  200-4</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA EL TOPETE  246</t>
   </si>
 </sst>
 </file>
@@ -4076,78 +4091,6 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4181,11 +4124,83 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4215,12 +4230,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4254,6 +4263,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4585,18 +4600,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="512" t="s">
+      <c r="A1" s="488" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
+      <c r="B1" s="488"/>
+      <c r="C1" s="488"/>
+      <c r="D1" s="488"/>
+      <c r="E1" s="488"/>
+      <c r="F1" s="488"/>
+      <c r="G1" s="488"/>
+      <c r="H1" s="488"/>
+      <c r="I1" s="488"/>
+      <c r="J1" s="488"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -4610,22 +4625,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="513" t="s">
+      <c r="W1" s="489" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="514"/>
+      <c r="X1" s="490"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="512"/>
-      <c r="B2" s="512"/>
-      <c r="C2" s="512"/>
-      <c r="D2" s="512"/>
-      <c r="E2" s="512"/>
-      <c r="F2" s="512"/>
-      <c r="G2" s="512"/>
-      <c r="H2" s="512"/>
-      <c r="I2" s="512"/>
-      <c r="J2" s="512"/>
+      <c r="A2" s="488"/>
+      <c r="B2" s="488"/>
+      <c r="C2" s="488"/>
+      <c r="D2" s="488"/>
+      <c r="E2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="488"/>
+      <c r="H2" s="488"/>
+      <c r="I2" s="488"/>
+      <c r="J2" s="488"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4679,10 +4694,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="515" t="s">
+      <c r="O3" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="516"/>
+      <c r="P3" s="492"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5226,7 +5241,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="517" t="s">
+      <c r="C12" s="493" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5290,7 +5305,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="518"/>
+      <c r="C13" s="494"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7292,13 +7307,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="496" t="s">
+      <c r="A56" s="505" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="498" t="s">
+      <c r="C56" s="507" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7309,7 +7324,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="500">
+      <c r="H56" s="499">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7338,11 +7353,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="497"/>
+      <c r="A57" s="506"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="499"/>
+      <c r="C57" s="508"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7351,7 +7366,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="501"/>
+      <c r="H57" s="500"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7378,13 +7393,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="496" t="s">
+      <c r="A58" s="505" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="498" t="s">
+      <c r="C58" s="507" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7395,7 +7410,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="500">
+      <c r="H58" s="499">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7414,10 +7429,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="502" t="s">
+      <c r="O58" s="501" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="523">
+      <c r="P58" s="503">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7428,11 +7443,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="497"/>
+      <c r="A59" s="506"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="499"/>
+      <c r="C59" s="508"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7441,7 +7456,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="501"/>
+      <c r="H59" s="500"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -7458,8 +7473,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="503"/>
-      <c r="P59" s="524"/>
+      <c r="O59" s="502"/>
+      <c r="P59" s="504"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7468,13 +7483,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="521" t="s">
+      <c r="A60" s="497" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="519" t="s">
+      <c r="C60" s="495" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -7488,7 +7503,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="500">
+      <c r="H60" s="499">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -7507,10 +7522,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="502" t="s">
+      <c r="O60" s="501" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="523">
+      <c r="P60" s="503">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -7523,11 +7538,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="522"/>
+      <c r="A61" s="498"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="520"/>
+      <c r="C61" s="496"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -7539,7 +7554,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="501"/>
+      <c r="H61" s="500"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -7556,8 +7571,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="503"/>
-      <c r="P61" s="524"/>
+      <c r="O61" s="502"/>
+      <c r="P61" s="504"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -7623,7 +7638,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="490"/>
+      <c r="C63" s="521"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7631,7 +7646,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="492"/>
+      <c r="H63" s="523"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7660,7 +7675,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="491"/>
+      <c r="C64" s="522"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7668,7 +7683,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="493"/>
+      <c r="H64" s="524"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -7846,8 +7861,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="494"/>
-      <c r="P68" s="488"/>
+      <c r="O68" s="513"/>
+      <c r="P68" s="519"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -7881,8 +7896,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="495"/>
-      <c r="P69" s="489"/>
+      <c r="O69" s="514"/>
+      <c r="P69" s="520"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8372,8 +8387,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="494"/>
-      <c r="P82" s="508"/>
+      <c r="O82" s="513"/>
+      <c r="P82" s="515"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8405,8 +8420,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="495"/>
-      <c r="P83" s="509"/>
+      <c r="O83" s="514"/>
+      <c r="P83" s="516"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8438,8 +8453,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="494"/>
-      <c r="P84" s="508"/>
+      <c r="O84" s="513"/>
+      <c r="P84" s="515"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8471,8 +8486,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="495"/>
-      <c r="P85" s="509"/>
+      <c r="O85" s="514"/>
+      <c r="P85" s="516"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8630,8 +8645,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="510"/>
-      <c r="M90" s="511"/>
+      <c r="L90" s="517"/>
+      <c r="M90" s="518"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8663,8 +8678,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="510"/>
-      <c r="M91" s="511"/>
+      <c r="L91" s="517"/>
+      <c r="M91" s="518"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8867,8 +8882,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="494"/>
-      <c r="P97" s="504"/>
+      <c r="O97" s="513"/>
+      <c r="P97" s="509"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -8900,8 +8915,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="495"/>
-      <c r="P98" s="505"/>
+      <c r="O98" s="514"/>
+      <c r="P98" s="510"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14293,11 +14308,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="506" t="s">
+      <c r="F262" s="511" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="506"/>
-      <c r="H262" s="507"/>
+      <c r="G262" s="511"/>
+      <c r="H262" s="512"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -14871,6 +14886,22 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -14884,22 +14915,6 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14943,18 +14958,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="512" t="s">
+      <c r="A1" s="488" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
+      <c r="B1" s="488"/>
+      <c r="C1" s="488"/>
+      <c r="D1" s="488"/>
+      <c r="E1" s="488"/>
+      <c r="F1" s="488"/>
+      <c r="G1" s="488"/>
+      <c r="H1" s="488"/>
+      <c r="I1" s="488"/>
+      <c r="J1" s="488"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -14970,22 +14985,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="513" t="s">
+      <c r="W1" s="489" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="514"/>
+      <c r="X1" s="490"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="512"/>
-      <c r="B2" s="512"/>
-      <c r="C2" s="512"/>
-      <c r="D2" s="512"/>
-      <c r="E2" s="512"/>
-      <c r="F2" s="512"/>
-      <c r="G2" s="512"/>
-      <c r="H2" s="512"/>
-      <c r="I2" s="512"/>
-      <c r="J2" s="512"/>
+      <c r="A2" s="488"/>
+      <c r="B2" s="488"/>
+      <c r="C2" s="488"/>
+      <c r="D2" s="488"/>
+      <c r="E2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="488"/>
+      <c r="H2" s="488"/>
+      <c r="I2" s="488"/>
+      <c r="J2" s="488"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -15039,10 +15054,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="515" t="s">
+      <c r="O3" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="516"/>
+      <c r="P3" s="492"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17684,7 +17699,7 @@
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="498" t="s">
+      <c r="C55" s="507" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17695,7 +17710,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="492" t="s">
+      <c r="H55" s="523" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -17728,7 +17743,7 @@
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="499"/>
+      <c r="C56" s="508"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -17737,7 +17752,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="493"/>
+      <c r="H56" s="524"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -17783,7 +17798,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="492" t="s">
+      <c r="H57" s="523" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -17802,10 +17817,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="494" t="s">
+      <c r="O57" s="513" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="488">
+      <c r="P57" s="519">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -17829,7 +17844,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="493"/>
+      <c r="H58" s="524"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -17873,7 +17888,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="492" t="s">
+      <c r="H59" s="523" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -17917,7 +17932,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="493"/>
+      <c r="H60" s="524"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -18580,8 +18595,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="494"/>
-      <c r="P79" s="508"/>
+      <c r="O79" s="513"/>
+      <c r="P79" s="515"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -18610,8 +18625,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="495"/>
-      <c r="P80" s="509"/>
+      <c r="O80" s="514"/>
+      <c r="P80" s="516"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18640,8 +18655,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="494"/>
-      <c r="P81" s="508"/>
+      <c r="O81" s="513"/>
+      <c r="P81" s="515"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18673,8 +18688,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="495"/>
-      <c r="P82" s="509"/>
+      <c r="O82" s="514"/>
+      <c r="P82" s="516"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -18832,8 +18847,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="510"/>
-      <c r="M87" s="511"/>
+      <c r="L87" s="517"/>
+      <c r="M87" s="518"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18865,8 +18880,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="510"/>
-      <c r="M88" s="511"/>
+      <c r="L88" s="517"/>
+      <c r="M88" s="518"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19069,8 +19084,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="494"/>
-      <c r="P94" s="504"/>
+      <c r="O94" s="513"/>
+      <c r="P94" s="509"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -19102,8 +19117,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="495"/>
-      <c r="P95" s="505"/>
+      <c r="O95" s="514"/>
+      <c r="P95" s="510"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -24495,11 +24510,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="506" t="s">
+      <c r="F259" s="511" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="506"/>
-      <c r="H259" s="507"/>
+      <c r="G259" s="511"/>
+      <c r="H259" s="512"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -25073,12 +25088,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -25094,6 +25103,12 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25140,18 +25155,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="512" t="s">
+      <c r="A1" s="488" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
+      <c r="B1" s="488"/>
+      <c r="C1" s="488"/>
+      <c r="D1" s="488"/>
+      <c r="E1" s="488"/>
+      <c r="F1" s="488"/>
+      <c r="G1" s="488"/>
+      <c r="H1" s="488"/>
+      <c r="I1" s="488"/>
+      <c r="J1" s="488"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -25167,22 +25182,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="513" t="s">
+      <c r="W1" s="489" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="514"/>
+      <c r="X1" s="490"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="512"/>
-      <c r="B2" s="512"/>
-      <c r="C2" s="512"/>
-      <c r="D2" s="512"/>
-      <c r="E2" s="512"/>
-      <c r="F2" s="512"/>
-      <c r="G2" s="512"/>
-      <c r="H2" s="512"/>
-      <c r="I2" s="512"/>
-      <c r="J2" s="512"/>
+      <c r="A2" s="488"/>
+      <c r="B2" s="488"/>
+      <c r="C2" s="488"/>
+      <c r="D2" s="488"/>
+      <c r="E2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="488"/>
+      <c r="H2" s="488"/>
+      <c r="I2" s="488"/>
+      <c r="J2" s="488"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25236,10 +25251,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="515" t="s">
+      <c r="O3" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="516"/>
+      <c r="P3" s="492"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28453,7 +28468,7 @@
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="498" t="s">
+      <c r="C55" s="507" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28464,7 +28479,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="538" t="s">
+      <c r="H55" s="536" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28483,10 +28498,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="494" t="s">
+      <c r="O55" s="513" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="488">
+      <c r="P55" s="519">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -28497,11 +28512,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="537"/>
+      <c r="A56" s="535"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="499"/>
+      <c r="C56" s="508"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -28510,7 +28525,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="539"/>
+      <c r="H56" s="537"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -28527,8 +28542,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="495"/>
-      <c r="P56" s="489"/>
+      <c r="O56" s="514"/>
+      <c r="P56" s="520"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -28589,13 +28604,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="521" t="s">
+      <c r="A58" s="497" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="535" t="s">
+      <c r="C58" s="546" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -28606,7 +28621,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="546" t="s">
+      <c r="H58" s="544" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -28625,10 +28640,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="502" t="s">
+      <c r="O58" s="501" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="523">
+      <c r="P58" s="503">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -28639,11 +28654,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="522"/>
+      <c r="A59" s="498"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="536"/>
+      <c r="C59" s="547"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -28652,7 +28667,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="547"/>
+      <c r="H59" s="545"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -28669,8 +28684,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="503"/>
-      <c r="P59" s="524"/>
+      <c r="O59" s="502"/>
+      <c r="P59" s="504"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -28743,13 +28758,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="540" t="s">
+      <c r="A62" s="538" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="542" t="s">
+      <c r="C62" s="540" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -28760,7 +28775,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="544">
+      <c r="H62" s="542">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -28779,10 +28794,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="494" t="s">
+      <c r="O62" s="513" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="488">
+      <c r="P62" s="519">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -28793,11 +28808,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="541"/>
+      <c r="A63" s="539"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="543"/>
+      <c r="C63" s="541"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -28806,7 +28821,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="545"/>
+      <c r="H63" s="543"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -28823,8 +28838,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="495"/>
-      <c r="P63" s="489"/>
+      <c r="O63" s="514"/>
+      <c r="P63" s="520"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29303,8 +29318,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="494"/>
-      <c r="P79" s="508"/>
+      <c r="O79" s="513"/>
+      <c r="P79" s="515"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29333,8 +29348,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="495"/>
-      <c r="P80" s="509"/>
+      <c r="O80" s="514"/>
+      <c r="P80" s="516"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29363,8 +29378,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="494"/>
-      <c r="P81" s="508"/>
+      <c r="O81" s="513"/>
+      <c r="P81" s="515"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29396,8 +29411,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="495"/>
-      <c r="P82" s="509"/>
+      <c r="O82" s="514"/>
+      <c r="P82" s="516"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -29555,8 +29570,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="510"/>
-      <c r="M87" s="511"/>
+      <c r="L87" s="517"/>
+      <c r="M87" s="518"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29588,8 +29603,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="510"/>
-      <c r="M88" s="511"/>
+      <c r="L88" s="517"/>
+      <c r="M88" s="518"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29792,8 +29807,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="494"/>
-      <c r="P94" s="504"/>
+      <c r="O94" s="513"/>
+      <c r="P94" s="509"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -29825,8 +29840,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="495"/>
-      <c r="P95" s="505"/>
+      <c r="O95" s="514"/>
+      <c r="P95" s="510"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35218,11 +35233,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="506" t="s">
+      <c r="F259" s="511" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="506"/>
-      <c r="H259" s="507"/>
+      <c r="G259" s="511"/>
+      <c r="H259" s="512"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -35796,6 +35811,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -35812,17 +35838,6 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35869,18 +35884,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="512" t="s">
+      <c r="A1" s="488" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
+      <c r="B1" s="488"/>
+      <c r="C1" s="488"/>
+      <c r="D1" s="488"/>
+      <c r="E1" s="488"/>
+      <c r="F1" s="488"/>
+      <c r="G1" s="488"/>
+      <c r="H1" s="488"/>
+      <c r="I1" s="488"/>
+      <c r="J1" s="488"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -35896,22 +35911,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="513" t="s">
+      <c r="W1" s="489" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="514"/>
+      <c r="X1" s="490"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="512"/>
-      <c r="B2" s="512"/>
-      <c r="C2" s="512"/>
-      <c r="D2" s="512"/>
-      <c r="E2" s="512"/>
-      <c r="F2" s="512"/>
-      <c r="G2" s="512"/>
-      <c r="H2" s="512"/>
-      <c r="I2" s="512"/>
-      <c r="J2" s="512"/>
+      <c r="A2" s="488"/>
+      <c r="B2" s="488"/>
+      <c r="C2" s="488"/>
+      <c r="D2" s="488"/>
+      <c r="E2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="488"/>
+      <c r="H2" s="488"/>
+      <c r="I2" s="488"/>
+      <c r="J2" s="488"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -35965,10 +35980,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="515" t="s">
+      <c r="O3" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="516"/>
+      <c r="P3" s="492"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -39764,8 +39779,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="494"/>
-      <c r="P79" s="508"/>
+      <c r="O79" s="513"/>
+      <c r="P79" s="515"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -39794,8 +39809,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="495"/>
-      <c r="P80" s="509"/>
+      <c r="O80" s="514"/>
+      <c r="P80" s="516"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -39824,8 +39839,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="494"/>
-      <c r="P81" s="508"/>
+      <c r="O81" s="513"/>
+      <c r="P81" s="515"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -39857,8 +39872,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="495"/>
-      <c r="P82" s="509"/>
+      <c r="O82" s="514"/>
+      <c r="P82" s="516"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -40016,8 +40031,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="510"/>
-      <c r="M87" s="511"/>
+      <c r="L87" s="517"/>
+      <c r="M87" s="518"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40049,8 +40064,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="510"/>
-      <c r="M88" s="511"/>
+      <c r="L88" s="517"/>
+      <c r="M88" s="518"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40253,8 +40268,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="494"/>
-      <c r="P94" s="504"/>
+      <c r="O94" s="513"/>
+      <c r="P94" s="509"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -40286,8 +40301,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="495"/>
-      <c r="P95" s="505"/>
+      <c r="O95" s="514"/>
+      <c r="P95" s="510"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -45679,11 +45694,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="506" t="s">
+      <c r="F259" s="511" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="506"/>
-      <c r="H259" s="507"/>
+      <c r="G259" s="511"/>
+      <c r="H259" s="512"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491156.35000000003</v>
@@ -46257,18 +46272,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="S1:T2"/>
     <mergeCell ref="F259:H259"/>
     <mergeCell ref="O81:O82"/>
     <mergeCell ref="P81:P82"/>
     <mergeCell ref="L87:M88"/>
     <mergeCell ref="O94:O95"/>
     <mergeCell ref="P94:P95"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="S1:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46283,10 +46298,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="I25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -46315,18 +46330,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="512" t="s">
+      <c r="A1" s="488" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
+      <c r="B1" s="488"/>
+      <c r="C1" s="488"/>
+      <c r="D1" s="488"/>
+      <c r="E1" s="488"/>
+      <c r="F1" s="488"/>
+      <c r="G1" s="488"/>
+      <c r="H1" s="488"/>
+      <c r="I1" s="488"/>
+      <c r="J1" s="488"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -46342,22 +46357,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="513" t="s">
+      <c r="W1" s="489" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="514"/>
+      <c r="X1" s="490"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="512"/>
-      <c r="B2" s="512"/>
-      <c r="C2" s="512"/>
-      <c r="D2" s="512"/>
-      <c r="E2" s="512"/>
-      <c r="F2" s="512"/>
-      <c r="G2" s="512"/>
-      <c r="H2" s="512"/>
-      <c r="I2" s="512"/>
-      <c r="J2" s="512"/>
+      <c r="A2" s="488"/>
+      <c r="B2" s="488"/>
+      <c r="C2" s="488"/>
+      <c r="D2" s="488"/>
+      <c r="E2" s="488"/>
+      <c r="F2" s="488"/>
+      <c r="G2" s="488"/>
+      <c r="H2" s="488"/>
+      <c r="I2" s="488"/>
+      <c r="J2" s="488"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -46411,10 +46426,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="515" t="s">
+      <c r="O3" s="491" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="516"/>
+      <c r="P3" s="492"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -47702,7 +47717,7 @@
     </row>
     <row r="24" spans="1:24" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="83" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="B24" s="58" t="s">
         <v>32</v>
@@ -47762,28 +47777,40 @@
       <c r="X24" s="70"/>
     </row>
     <row r="25" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="71"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="71" t="s">
+        <v>462</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>463</v>
+      </c>
       <c r="C25" s="59"/>
       <c r="D25" s="60"/>
       <c r="E25" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="62"/>
+      <c r="F25" s="61">
+        <v>21430</v>
+      </c>
+      <c r="G25" s="62">
+        <v>44703</v>
+      </c>
       <c r="H25" s="410"/>
-      <c r="I25" s="411"/>
+      <c r="I25" s="411">
+        <v>22170</v>
+      </c>
       <c r="J25" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="76"/>
+        <v>740</v>
+      </c>
+      <c r="K25" s="76">
+        <v>37</v>
+      </c>
       <c r="L25" s="65"/>
       <c r="M25" s="65"/>
       <c r="N25" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>820290</v>
       </c>
       <c r="O25" s="89"/>
       <c r="P25" s="90"/>
@@ -47797,28 +47824,40 @@
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="82"/>
-      <c r="B26" s="58"/>
+      <c r="A26" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>32</v>
+      </c>
       <c r="C26" s="59"/>
       <c r="D26" s="60"/>
       <c r="E26" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26" s="61"/>
-      <c r="G26" s="62"/>
+      <c r="F26" s="61">
+        <v>0</v>
+      </c>
+      <c r="G26" s="62">
+        <v>44703</v>
+      </c>
       <c r="H26" s="410"/>
-      <c r="I26" s="411"/>
+      <c r="I26" s="411">
+        <v>5385</v>
+      </c>
       <c r="J26" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="76"/>
+        <v>5385</v>
+      </c>
+      <c r="K26" s="76">
+        <v>37</v>
+      </c>
       <c r="L26" s="65"/>
       <c r="M26" s="65"/>
       <c r="N26" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>199245</v>
       </c>
       <c r="O26" s="89"/>
       <c r="P26" s="90"/>
@@ -47832,28 +47871,40 @@
       <c r="X26" s="70"/>
     </row>
     <row r="27" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="82"/>
-      <c r="B27" s="58"/>
+      <c r="A27" s="82" t="s">
+        <v>464</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>465</v>
+      </c>
       <c r="C27" s="59"/>
       <c r="D27" s="60"/>
       <c r="E27" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
+      <c r="F27" s="61">
+        <v>20950</v>
+      </c>
+      <c r="G27" s="62">
+        <v>44705</v>
+      </c>
       <c r="H27" s="410"/>
-      <c r="I27" s="411"/>
+      <c r="I27" s="411">
+        <v>21470</v>
+      </c>
       <c r="J27" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="76"/>
+        <v>520</v>
+      </c>
+      <c r="K27" s="76">
+        <v>37</v>
+      </c>
       <c r="L27" s="65"/>
       <c r="M27" s="65"/>
       <c r="N27" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>794390</v>
       </c>
       <c r="O27" s="89"/>
       <c r="P27" s="90"/>
@@ -47867,28 +47918,40 @@
       <c r="X27" s="70"/>
     </row>
     <row r="28" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="82"/>
-      <c r="B28" s="58"/>
+      <c r="A28" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>32</v>
+      </c>
       <c r="C28" s="59"/>
       <c r="D28" s="60"/>
       <c r="E28" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
+      <c r="F28" s="61">
+        <v>0</v>
+      </c>
+      <c r="G28" s="62">
+        <v>44705</v>
+      </c>
       <c r="H28" s="410"/>
-      <c r="I28" s="411"/>
+      <c r="I28" s="411">
+        <v>5535</v>
+      </c>
       <c r="J28" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="76"/>
+        <v>5535</v>
+      </c>
+      <c r="K28" s="76">
+        <v>37</v>
+      </c>
       <c r="L28" s="65"/>
       <c r="M28" s="65"/>
       <c r="N28" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>204795</v>
       </c>
       <c r="O28" s="89"/>
       <c r="P28" s="90"/>
@@ -47902,28 +47965,40 @@
       <c r="X28" s="70"/>
     </row>
     <row r="29" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57"/>
-      <c r="B29" s="93"/>
+      <c r="A29" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="93" t="s">
+        <v>290</v>
+      </c>
       <c r="C29" s="59"/>
       <c r="D29" s="60"/>
       <c r="E29" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
+      <c r="F29" s="61">
+        <v>22190</v>
+      </c>
+      <c r="G29" s="62">
+        <v>44707</v>
+      </c>
       <c r="H29" s="410"/>
-      <c r="I29" s="411"/>
+      <c r="I29" s="411">
+        <v>22070</v>
+      </c>
       <c r="J29" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="76"/>
+        <v>-120</v>
+      </c>
+      <c r="K29" s="76">
+        <v>37.5</v>
+      </c>
       <c r="L29" s="65"/>
       <c r="M29" s="65"/>
       <c r="N29" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>827625</v>
       </c>
       <c r="O29" s="89"/>
       <c r="P29" s="90"/>
@@ -47937,28 +48012,40 @@
       <c r="X29" s="70"/>
     </row>
     <row r="30" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="57"/>
-      <c r="B30" s="93"/>
+      <c r="A30" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="93" t="s">
+        <v>32</v>
+      </c>
       <c r="C30" s="59"/>
       <c r="D30" s="60"/>
       <c r="E30" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F30" s="61"/>
-      <c r="G30" s="62"/>
+      <c r="F30" s="61">
+        <v>0</v>
+      </c>
+      <c r="G30" s="62">
+        <v>44707</v>
+      </c>
       <c r="H30" s="410"/>
-      <c r="I30" s="411"/>
+      <c r="I30" s="411">
+        <v>5870</v>
+      </c>
       <c r="J30" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="76"/>
+        <v>5870</v>
+      </c>
+      <c r="K30" s="76">
+        <v>37.5</v>
+      </c>
       <c r="L30" s="65"/>
       <c r="M30" s="65"/>
       <c r="N30" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>220125</v>
       </c>
       <c r="O30" s="89"/>
       <c r="P30" s="90"/>
@@ -47971,29 +48058,41 @@
       <c r="W30" s="53"/>
       <c r="X30" s="70"/>
     </row>
-    <row r="31" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="71"/>
-      <c r="B31" s="93"/>
+    <row r="31" spans="1:24" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="93" t="s">
+        <v>72</v>
+      </c>
       <c r="C31" s="59"/>
       <c r="D31" s="60"/>
       <c r="E31" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F31" s="61"/>
-      <c r="G31" s="62"/>
+      <c r="F31" s="61">
+        <v>22690</v>
+      </c>
+      <c r="G31" s="62">
+        <v>44708</v>
+      </c>
       <c r="H31" s="410"/>
-      <c r="I31" s="411"/>
+      <c r="I31" s="411">
+        <v>22530</v>
+      </c>
       <c r="J31" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="76"/>
+        <v>-160</v>
+      </c>
+      <c r="K31" s="76">
+        <v>38</v>
+      </c>
       <c r="L31" s="65"/>
       <c r="M31" s="65"/>
       <c r="N31" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>856140</v>
       </c>
       <c r="O31" s="89"/>
       <c r="P31" s="90"/>
@@ -48006,29 +48105,41 @@
       <c r="W31" s="53"/>
       <c r="X31" s="70"/>
     </row>
-    <row r="32" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="71"/>
-      <c r="B32" s="93"/>
+    <row r="32" spans="1:24" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="93" t="s">
+        <v>32</v>
+      </c>
       <c r="C32" s="59"/>
       <c r="D32" s="60"/>
       <c r="E32" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F32" s="61"/>
-      <c r="G32" s="62"/>
+      <c r="F32" s="61">
+        <v>0</v>
+      </c>
+      <c r="G32" s="62">
+        <v>44708</v>
+      </c>
       <c r="H32" s="410"/>
-      <c r="I32" s="411"/>
+      <c r="I32" s="411">
+        <v>5930</v>
+      </c>
       <c r="J32" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="76"/>
+        <v>5930</v>
+      </c>
+      <c r="K32" s="76">
+        <v>38</v>
+      </c>
       <c r="L32" s="65"/>
       <c r="M32" s="65"/>
       <c r="N32" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>225340</v>
       </c>
       <c r="O32" s="98"/>
       <c r="P32" s="90"/>
@@ -48042,28 +48153,40 @@
       <c r="X32" s="70"/>
     </row>
     <row r="33" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="83"/>
-      <c r="B33" s="93"/>
+      <c r="A33" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="B33" s="93" t="s">
+        <v>290</v>
+      </c>
       <c r="C33" s="59"/>
       <c r="D33" s="60"/>
       <c r="E33" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F33" s="61"/>
-      <c r="G33" s="62"/>
+      <c r="F33" s="61">
+        <v>21001</v>
+      </c>
+      <c r="G33" s="62">
+        <v>44710</v>
+      </c>
       <c r="H33" s="410"/>
-      <c r="I33" s="411"/>
+      <c r="I33" s="411">
+        <v>21360</v>
+      </c>
       <c r="J33" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="76"/>
+        <v>359</v>
+      </c>
+      <c r="K33" s="76">
+        <v>38.5</v>
+      </c>
       <c r="L33" s="99"/>
       <c r="M33" s="99"/>
       <c r="N33" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>822360</v>
       </c>
       <c r="O33" s="98"/>
       <c r="P33" s="90"/>
@@ -48076,29 +48199,41 @@
       <c r="W33" s="53"/>
       <c r="X33" s="70"/>
     </row>
-    <row r="34" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="82"/>
-      <c r="B34" s="93"/>
+    <row r="34" spans="1:24" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="93" t="s">
+        <v>32</v>
+      </c>
       <c r="C34" s="59"/>
       <c r="D34" s="60"/>
       <c r="E34" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F34" s="61"/>
-      <c r="G34" s="62"/>
+      <c r="F34" s="61">
+        <v>0</v>
+      </c>
+      <c r="G34" s="62">
+        <v>44710</v>
+      </c>
       <c r="H34" s="410"/>
-      <c r="I34" s="411"/>
+      <c r="I34" s="411">
+        <v>5355</v>
+      </c>
       <c r="J34" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="76"/>
+        <v>5355</v>
+      </c>
+      <c r="K34" s="76">
+        <v>50</v>
+      </c>
       <c r="L34" s="99"/>
       <c r="M34" s="99"/>
       <c r="N34" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>267750</v>
       </c>
       <c r="O34" s="98"/>
       <c r="P34" s="90"/>
@@ -49811,8 +49946,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="510"/>
-      <c r="M87" s="511"/>
+      <c r="L87" s="517"/>
+      <c r="M87" s="518"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -49844,8 +49979,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="510"/>
-      <c r="M88" s="511"/>
+      <c r="L88" s="517"/>
+      <c r="M88" s="518"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50048,8 +50183,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="494"/>
-      <c r="P94" s="504"/>
+      <c r="O94" s="513"/>
+      <c r="P94" s="509"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -50081,8 +50216,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="495"/>
-      <c r="P95" s="505"/>
+      <c r="O95" s="514"/>
+      <c r="P95" s="510"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -55474,14 +55609,14 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="506" t="s">
+      <c r="F259" s="511" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="506"/>
-      <c r="H259" s="507"/>
+      <c r="G259" s="511"/>
+      <c r="H259" s="512"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
-        <v>316015</v>
+        <v>453690</v>
       </c>
       <c r="J259" s="318"/>
       <c r="K259" s="314"/>
@@ -55580,7 +55715,7 @@
       <c r="M263" s="336"/>
       <c r="N263" s="337">
         <f>SUM(N4:N262)</f>
-        <v>11272772.5</v>
+        <v>16510832.5</v>
       </c>
       <c r="O263" s="338"/>
       <c r="Q263" s="339">
@@ -55640,7 +55775,7 @@
       <c r="M266" s="352"/>
       <c r="N266" s="353">
         <f>V263+S263+Q263+N263+L263</f>
-        <v>11624208.5</v>
+        <v>16862268.5</v>
       </c>
       <c r="O266" s="354"/>
       <c r="R266" s="324"/>

</xml_diff>

<commit_message>
CIERRE 3 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/ENTRADAS OBRADOR     M A Y O        2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/ENTRADAS OBRADOR     M A Y O        2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16365" windowHeight="10305" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CANALES  ENERO  2022   " sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="482">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -1485,6 +1485,9 @@
   </si>
   <si>
     <t>A-928</t>
+  </si>
+  <si>
+    <t>D-4271</t>
   </si>
 </sst>
 </file>
@@ -4220,78 +4223,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4325,11 +4256,83 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4359,12 +4362,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4400,6 +4397,12 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="32" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4427,8 +4430,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FF0000FF"/>
-      <color rgb="FFFFCCFF"/>
       <color rgb="FFFF5050"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFCCFF33"/>
@@ -4747,18 +4750,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="533" t="s">
+      <c r="A1" s="509" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="533"/>
-      <c r="C1" s="533"/>
-      <c r="D1" s="533"/>
-      <c r="E1" s="533"/>
-      <c r="F1" s="533"/>
-      <c r="G1" s="533"/>
-      <c r="H1" s="533"/>
-      <c r="I1" s="533"/>
-      <c r="J1" s="533"/>
+      <c r="B1" s="509"/>
+      <c r="C1" s="509"/>
+      <c r="D1" s="509"/>
+      <c r="E1" s="509"/>
+      <c r="F1" s="509"/>
+      <c r="G1" s="509"/>
+      <c r="H1" s="509"/>
+      <c r="I1" s="509"/>
+      <c r="J1" s="509"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -4772,22 +4775,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="534" t="s">
+      <c r="W1" s="510" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="535"/>
+      <c r="X1" s="511"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="533"/>
-      <c r="B2" s="533"/>
-      <c r="C2" s="533"/>
-      <c r="D2" s="533"/>
-      <c r="E2" s="533"/>
-      <c r="F2" s="533"/>
-      <c r="G2" s="533"/>
-      <c r="H2" s="533"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="533"/>
+      <c r="A2" s="509"/>
+      <c r="B2" s="509"/>
+      <c r="C2" s="509"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="509"/>
+      <c r="F2" s="509"/>
+      <c r="G2" s="509"/>
+      <c r="H2" s="509"/>
+      <c r="I2" s="509"/>
+      <c r="J2" s="509"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4841,10 +4844,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="536" t="s">
+      <c r="O3" s="512" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="537"/>
+      <c r="P3" s="513"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -5388,7 +5391,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="538" t="s">
+      <c r="C12" s="514" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -5452,7 +5455,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="539"/>
+      <c r="C13" s="515"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -7454,13 +7457,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="517" t="s">
+      <c r="A56" s="526" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="519" t="s">
+      <c r="C56" s="528" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -7471,7 +7474,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="521">
+      <c r="H56" s="520">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -7500,11 +7503,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="518"/>
+      <c r="A57" s="527"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="520"/>
+      <c r="C57" s="529"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -7513,7 +7516,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="522"/>
+      <c r="H57" s="521"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -7540,13 +7543,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="517" t="s">
+      <c r="A58" s="526" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="519" t="s">
+      <c r="C58" s="528" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -7557,7 +7560,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="521">
+      <c r="H58" s="520">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -7576,10 +7579,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="523" t="s">
+      <c r="O58" s="522" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="544">
+      <c r="P58" s="524">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -7590,11 +7593,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="518"/>
+      <c r="A59" s="527"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="520"/>
+      <c r="C59" s="529"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -7603,7 +7606,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="522"/>
+      <c r="H59" s="521"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -7620,8 +7623,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="524"/>
-      <c r="P59" s="545"/>
+      <c r="O59" s="523"/>
+      <c r="P59" s="525"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -7630,13 +7633,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="542" t="s">
+      <c r="A60" s="518" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="540" t="s">
+      <c r="C60" s="516" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -7650,7 +7653,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="521">
+      <c r="H60" s="520">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -7669,10 +7672,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="523" t="s">
+      <c r="O60" s="522" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="544">
+      <c r="P60" s="524">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -7685,11 +7688,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="543"/>
+      <c r="A61" s="519"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="541"/>
+      <c r="C61" s="517"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -7701,7 +7704,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="522"/>
+      <c r="H61" s="521"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -7718,8 +7721,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="524"/>
-      <c r="P61" s="545"/>
+      <c r="O61" s="523"/>
+      <c r="P61" s="525"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -7785,7 +7788,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="511"/>
+      <c r="C63" s="542"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7793,7 +7796,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="513"/>
+      <c r="H63" s="544"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7822,7 +7825,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="512"/>
+      <c r="C64" s="543"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7830,7 +7833,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="514"/>
+      <c r="H64" s="545"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -8008,8 +8011,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="515"/>
-      <c r="P68" s="509"/>
+      <c r="O68" s="534"/>
+      <c r="P68" s="540"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -8043,8 +8046,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="516"/>
-      <c r="P69" s="510"/>
+      <c r="O69" s="535"/>
+      <c r="P69" s="541"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -8534,8 +8537,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="515"/>
-      <c r="P82" s="529"/>
+      <c r="O82" s="534"/>
+      <c r="P82" s="536"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -8567,8 +8570,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="516"/>
-      <c r="P83" s="530"/>
+      <c r="O83" s="535"/>
+      <c r="P83" s="537"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -8600,8 +8603,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="515"/>
-      <c r="P84" s="529"/>
+      <c r="O84" s="534"/>
+      <c r="P84" s="536"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -8633,8 +8636,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="516"/>
-      <c r="P85" s="530"/>
+      <c r="O85" s="535"/>
+      <c r="P85" s="537"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8792,8 +8795,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="531"/>
-      <c r="M90" s="532"/>
+      <c r="L90" s="538"/>
+      <c r="M90" s="539"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8825,8 +8828,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="531"/>
-      <c r="M91" s="532"/>
+      <c r="L91" s="538"/>
+      <c r="M91" s="539"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -9029,8 +9032,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="515"/>
-      <c r="P97" s="525"/>
+      <c r="O97" s="534"/>
+      <c r="P97" s="530"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -9062,8 +9065,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="516"/>
-      <c r="P98" s="526"/>
+      <c r="O98" s="535"/>
+      <c r="P98" s="531"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -14455,11 +14458,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="527" t="s">
+      <c r="F262" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="527"/>
-      <c r="H262" s="528"/>
+      <c r="G262" s="532"/>
+      <c r="H262" s="533"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -15033,6 +15036,22 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -15046,22 +15065,6 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15105,18 +15108,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="533" t="s">
+      <c r="A1" s="509" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="533"/>
-      <c r="C1" s="533"/>
-      <c r="D1" s="533"/>
-      <c r="E1" s="533"/>
-      <c r="F1" s="533"/>
-      <c r="G1" s="533"/>
-      <c r="H1" s="533"/>
-      <c r="I1" s="533"/>
-      <c r="J1" s="533"/>
+      <c r="B1" s="509"/>
+      <c r="C1" s="509"/>
+      <c r="D1" s="509"/>
+      <c r="E1" s="509"/>
+      <c r="F1" s="509"/>
+      <c r="G1" s="509"/>
+      <c r="H1" s="509"/>
+      <c r="I1" s="509"/>
+      <c r="J1" s="509"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -15132,22 +15135,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="534" t="s">
+      <c r="W1" s="510" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="535"/>
+      <c r="X1" s="511"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="533"/>
-      <c r="B2" s="533"/>
-      <c r="C2" s="533"/>
-      <c r="D2" s="533"/>
-      <c r="E2" s="533"/>
-      <c r="F2" s="533"/>
-      <c r="G2" s="533"/>
-      <c r="H2" s="533"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="533"/>
+      <c r="A2" s="509"/>
+      <c r="B2" s="509"/>
+      <c r="C2" s="509"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="509"/>
+      <c r="F2" s="509"/>
+      <c r="G2" s="509"/>
+      <c r="H2" s="509"/>
+      <c r="I2" s="509"/>
+      <c r="J2" s="509"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -15201,10 +15204,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="536" t="s">
+      <c r="O3" s="512" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="537"/>
+      <c r="P3" s="513"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17846,7 +17849,7 @@
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="519" t="s">
+      <c r="C55" s="528" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17857,7 +17860,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="513" t="s">
+      <c r="H55" s="544" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -17890,7 +17893,7 @@
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="520"/>
+      <c r="C56" s="529"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -17899,7 +17902,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="514"/>
+      <c r="H56" s="545"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -17945,7 +17948,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="513" t="s">
+      <c r="H57" s="544" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -17964,10 +17967,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="515" t="s">
+      <c r="O57" s="534" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="509">
+      <c r="P57" s="540">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -17991,7 +17994,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="514"/>
+      <c r="H58" s="545"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -18035,7 +18038,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="513" t="s">
+      <c r="H59" s="544" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="151">
@@ -18079,7 +18082,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="514"/>
+      <c r="H60" s="545"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -18742,8 +18745,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="515"/>
-      <c r="P79" s="529"/>
+      <c r="O79" s="534"/>
+      <c r="P79" s="536"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -18772,8 +18775,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="516"/>
-      <c r="P80" s="530"/>
+      <c r="O80" s="535"/>
+      <c r="P80" s="537"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18802,8 +18805,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="515"/>
-      <c r="P81" s="529"/>
+      <c r="O81" s="534"/>
+      <c r="P81" s="536"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18835,8 +18838,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="516"/>
-      <c r="P82" s="530"/>
+      <c r="O82" s="535"/>
+      <c r="P82" s="537"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -18994,8 +18997,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="531"/>
-      <c r="M87" s="532"/>
+      <c r="L87" s="538"/>
+      <c r="M87" s="539"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19027,8 +19030,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="531"/>
-      <c r="M88" s="532"/>
+      <c r="L88" s="538"/>
+      <c r="M88" s="539"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -19231,8 +19234,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="515"/>
-      <c r="P94" s="525"/>
+      <c r="O94" s="534"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -19264,8 +19267,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="516"/>
-      <c r="P95" s="526"/>
+      <c r="O95" s="535"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -24657,11 +24660,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="527" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="527"/>
-      <c r="H259" s="528"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -25235,12 +25238,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -25256,6 +25253,12 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -25302,18 +25305,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="533" t="s">
+      <c r="A1" s="509" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="533"/>
-      <c r="C1" s="533"/>
-      <c r="D1" s="533"/>
-      <c r="E1" s="533"/>
-      <c r="F1" s="533"/>
-      <c r="G1" s="533"/>
-      <c r="H1" s="533"/>
-      <c r="I1" s="533"/>
-      <c r="J1" s="533"/>
+      <c r="B1" s="509"/>
+      <c r="C1" s="509"/>
+      <c r="D1" s="509"/>
+      <c r="E1" s="509"/>
+      <c r="F1" s="509"/>
+      <c r="G1" s="509"/>
+      <c r="H1" s="509"/>
+      <c r="I1" s="509"/>
+      <c r="J1" s="509"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -25329,22 +25332,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="534" t="s">
+      <c r="W1" s="510" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="535"/>
+      <c r="X1" s="511"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="533"/>
-      <c r="B2" s="533"/>
-      <c r="C2" s="533"/>
-      <c r="D2" s="533"/>
-      <c r="E2" s="533"/>
-      <c r="F2" s="533"/>
-      <c r="G2" s="533"/>
-      <c r="H2" s="533"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="533"/>
+      <c r="A2" s="509"/>
+      <c r="B2" s="509"/>
+      <c r="C2" s="509"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="509"/>
+      <c r="F2" s="509"/>
+      <c r="G2" s="509"/>
+      <c r="H2" s="509"/>
+      <c r="I2" s="509"/>
+      <c r="J2" s="509"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -25398,10 +25401,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="536" t="s">
+      <c r="O3" s="512" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="537"/>
+      <c r="P3" s="513"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -28615,7 +28618,7 @@
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="519" t="s">
+      <c r="C55" s="528" t="s">
         <v>229</v>
       </c>
       <c r="D55" s="439"/>
@@ -28626,7 +28629,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="559" t="s">
+      <c r="H55" s="557" t="s">
         <v>230</v>
       </c>
       <c r="I55" s="151">
@@ -28645,10 +28648,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="515" t="s">
+      <c r="O55" s="534" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="509">
+      <c r="P55" s="540">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -28659,11 +28662,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="558"/>
+      <c r="A56" s="556"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="520"/>
+      <c r="C56" s="529"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -28672,7 +28675,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="560"/>
+      <c r="H56" s="558"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -28689,8 +28692,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="516"/>
-      <c r="P56" s="510"/>
+      <c r="O56" s="535"/>
+      <c r="P56" s="541"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -28751,13 +28754,13 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="542" t="s">
+      <c r="A58" s="518" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="556" t="s">
+      <c r="C58" s="567" t="s">
         <v>319</v>
       </c>
       <c r="D58" s="165"/>
@@ -28768,7 +28771,7 @@
       <c r="G58" s="152">
         <v>44648</v>
       </c>
-      <c r="H58" s="567" t="s">
+      <c r="H58" s="565" t="s">
         <v>315</v>
       </c>
       <c r="I58" s="151">
@@ -28787,10 +28790,10 @@
         <f t="shared" si="1"/>
         <v>35255.600000000006</v>
       </c>
-      <c r="O58" s="523" t="s">
+      <c r="O58" s="522" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="544">
+      <c r="P58" s="524">
         <v>44662</v>
       </c>
       <c r="Q58" s="164"/>
@@ -28801,11 +28804,11 @@
       <c r="V58" s="54"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="543"/>
+      <c r="A59" s="519"/>
       <c r="B59" s="170" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="557"/>
+      <c r="C59" s="568"/>
       <c r="D59" s="163"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151">
@@ -28814,7 +28817,7 @@
       <c r="G59" s="152">
         <v>44648</v>
       </c>
-      <c r="H59" s="568"/>
+      <c r="H59" s="566"/>
       <c r="I59" s="151">
         <v>719</v>
       </c>
@@ -28831,8 +28834,8 @@
         <f t="shared" si="1"/>
         <v>69024</v>
       </c>
-      <c r="O59" s="524"/>
-      <c r="P59" s="545"/>
+      <c r="O59" s="523"/>
+      <c r="P59" s="525"/>
       <c r="Q59" s="164"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -28905,13 +28908,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="561" t="s">
+      <c r="A62" s="559" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="563" t="s">
+      <c r="C62" s="561" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="168"/>
@@ -28922,7 +28925,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="565">
+      <c r="H62" s="563">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -28941,10 +28944,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="515" t="s">
+      <c r="O62" s="534" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="509">
+      <c r="P62" s="540">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -28955,11 +28958,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="562"/>
+      <c r="A63" s="560"/>
       <c r="B63" s="178" t="s">
         <v>239</v>
       </c>
-      <c r="C63" s="564"/>
+      <c r="C63" s="562"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -28968,7 +28971,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="566"/>
+      <c r="H63" s="564"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -28985,8 +28988,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="516"/>
-      <c r="P63" s="510"/>
+      <c r="O63" s="535"/>
+      <c r="P63" s="541"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -29465,8 +29468,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="515"/>
-      <c r="P79" s="529"/>
+      <c r="O79" s="534"/>
+      <c r="P79" s="536"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -29495,8 +29498,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="516"/>
-      <c r="P80" s="530"/>
+      <c r="O80" s="535"/>
+      <c r="P80" s="537"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -29525,8 +29528,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="515"/>
-      <c r="P81" s="529"/>
+      <c r="O81" s="534"/>
+      <c r="P81" s="536"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -29558,8 +29561,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="516"/>
-      <c r="P82" s="530"/>
+      <c r="O82" s="535"/>
+      <c r="P82" s="537"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -29717,8 +29720,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="531"/>
-      <c r="M87" s="532"/>
+      <c r="L87" s="538"/>
+      <c r="M87" s="539"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29750,8 +29753,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="531"/>
-      <c r="M88" s="532"/>
+      <c r="L88" s="538"/>
+      <c r="M88" s="539"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29954,8 +29957,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="515"/>
-      <c r="P94" s="525"/>
+      <c r="O94" s="534"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -29987,8 +29990,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="516"/>
-      <c r="P95" s="526"/>
+      <c r="O95" s="535"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -35380,11 +35383,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="527" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="527"/>
-      <c r="H259" s="528"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>517031.52999999991</v>
@@ -35958,6 +35961,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P58:P59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -35974,17 +35988,6 @@
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
     <mergeCell ref="H58:H59"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P58:P59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35998,11 +36001,11 @@
   </sheetPr>
   <dimension ref="A1:X292"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="3" topLeftCell="O55" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="3" topLeftCell="U18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O67" sqref="O67"/>
+      <selection pane="bottomRight" activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -36031,18 +36034,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="533" t="s">
+      <c r="A1" s="509" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="533"/>
-      <c r="C1" s="533"/>
-      <c r="D1" s="533"/>
-      <c r="E1" s="533"/>
-      <c r="F1" s="533"/>
-      <c r="G1" s="533"/>
-      <c r="H1" s="533"/>
-      <c r="I1" s="533"/>
-      <c r="J1" s="533"/>
+      <c r="B1" s="509"/>
+      <c r="C1" s="509"/>
+      <c r="D1" s="509"/>
+      <c r="E1" s="509"/>
+      <c r="F1" s="509"/>
+      <c r="G1" s="509"/>
+      <c r="H1" s="509"/>
+      <c r="I1" s="509"/>
+      <c r="J1" s="509"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -36058,22 +36061,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="534" t="s">
+      <c r="W1" s="510" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="535"/>
+      <c r="X1" s="511"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="533"/>
-      <c r="B2" s="533"/>
-      <c r="C2" s="533"/>
-      <c r="D2" s="533"/>
-      <c r="E2" s="533"/>
-      <c r="F2" s="533"/>
-      <c r="G2" s="533"/>
-      <c r="H2" s="533"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="533"/>
+      <c r="A2" s="509"/>
+      <c r="B2" s="509"/>
+      <c r="C2" s="509"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="509"/>
+      <c r="F2" s="509"/>
+      <c r="G2" s="509"/>
+      <c r="H2" s="509"/>
+      <c r="I2" s="509"/>
+      <c r="J2" s="509"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -36127,10 +36130,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="536" t="s">
+      <c r="O3" s="512" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="537"/>
+      <c r="P3" s="513"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -37574,8 +37577,12 @@
       <c r="T23" s="92" t="s">
         <v>343</v>
       </c>
-      <c r="U23" s="53"/>
-      <c r="V23" s="54"/>
+      <c r="U23" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V23" s="479">
+        <v>4640</v>
+      </c>
       <c r="W23" s="53" t="s">
         <v>414</v>
       </c>
@@ -37644,8 +37651,12 @@
       <c r="T24" s="92" t="s">
         <v>343</v>
       </c>
-      <c r="U24" s="53"/>
-      <c r="V24" s="54"/>
+      <c r="U24" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V24" s="479">
+        <v>0</v>
+      </c>
       <c r="W24" s="53" t="s">
         <v>414</v>
       </c>
@@ -37653,7 +37664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="71" t="s">
         <v>341</v>
       </c>
@@ -37713,8 +37724,12 @@
       <c r="T25" s="92" t="s">
         <v>346</v>
       </c>
-      <c r="U25" s="53"/>
-      <c r="V25" s="54"/>
+      <c r="U25" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V25" s="479">
+        <v>4640</v>
+      </c>
       <c r="W25" s="53" t="s">
         <v>414</v>
       </c>
@@ -37783,8 +37798,12 @@
       <c r="T26" s="92" t="s">
         <v>346</v>
       </c>
-      <c r="U26" s="53"/>
-      <c r="V26" s="54"/>
+      <c r="U26" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V26" s="479">
+        <v>0</v>
+      </c>
       <c r="W26" s="53" t="s">
         <v>414</v>
       </c>
@@ -37853,8 +37872,12 @@
       <c r="T27" s="92" t="s">
         <v>386</v>
       </c>
-      <c r="U27" s="53"/>
-      <c r="V27" s="54"/>
+      <c r="U27" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V27" s="479">
+        <v>4640</v>
+      </c>
       <c r="W27" s="53" t="s">
         <v>414</v>
       </c>
@@ -37862,7 +37885,7 @@
         <v>4176</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="82" t="s">
         <v>223</v>
       </c>
@@ -37922,8 +37945,12 @@
       <c r="T28" s="92" t="s">
         <v>386</v>
       </c>
-      <c r="U28" s="53"/>
-      <c r="V28" s="54"/>
+      <c r="U28" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V28" s="479">
+        <v>0</v>
+      </c>
       <c r="W28" s="53" t="s">
         <v>414</v>
       </c>
@@ -37991,8 +38018,12 @@
       <c r="T29" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="U29" s="53"/>
-      <c r="V29" s="54"/>
+      <c r="U29" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V29" s="479">
+        <v>4640</v>
+      </c>
       <c r="W29" s="53" t="s">
         <v>414</v>
       </c>
@@ -38060,8 +38091,12 @@
       <c r="T30" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="U30" s="53"/>
-      <c r="V30" s="54"/>
+      <c r="U30" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V30" s="479">
+        <v>0</v>
+      </c>
       <c r="W30" s="53" t="s">
         <v>414</v>
       </c>
@@ -38125,8 +38160,12 @@
       </c>
       <c r="S31" s="91"/>
       <c r="T31" s="92"/>
-      <c r="U31" s="53"/>
-      <c r="V31" s="54"/>
+      <c r="U31" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V31" s="479">
+        <v>4640</v>
+      </c>
       <c r="W31" s="53" t="s">
         <v>414</v>
       </c>
@@ -38190,8 +38229,12 @@
       </c>
       <c r="S32" s="91"/>
       <c r="T32" s="92"/>
-      <c r="U32" s="53"/>
-      <c r="V32" s="54"/>
+      <c r="U32" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V32" s="479">
+        <v>0</v>
+      </c>
       <c r="W32" s="53" t="s">
         <v>414</v>
       </c>
@@ -38199,7 +38242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="83" t="s">
         <v>20</v>
       </c>
@@ -38259,8 +38302,12 @@
       <c r="T33" s="92" t="s">
         <v>389</v>
       </c>
-      <c r="U33" s="53"/>
-      <c r="V33" s="54"/>
+      <c r="U33" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V33" s="479">
+        <v>4640</v>
+      </c>
       <c r="W33" s="53" t="s">
         <v>414</v>
       </c>
@@ -38328,8 +38375,12 @@
       <c r="T34" s="92" t="s">
         <v>389</v>
       </c>
-      <c r="U34" s="53"/>
-      <c r="V34" s="54"/>
+      <c r="U34" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V34" s="479">
+        <v>0</v>
+      </c>
       <c r="W34" s="53" t="s">
         <v>414</v>
       </c>
@@ -38397,8 +38448,12 @@
       <c r="T35" s="92" t="s">
         <v>391</v>
       </c>
-      <c r="U35" s="53"/>
-      <c r="V35" s="54"/>
+      <c r="U35" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V35" s="479">
+        <v>4640</v>
+      </c>
       <c r="W35" s="53" t="s">
         <v>414</v>
       </c>
@@ -38406,7 +38461,7 @@
         <v>4176</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="57" t="s">
         <v>223</v>
       </c>
@@ -38464,8 +38519,12 @@
       <c r="T36" s="92" t="s">
         <v>391</v>
       </c>
-      <c r="U36" s="53"/>
-      <c r="V36" s="54"/>
+      <c r="U36" s="478" t="s">
+        <v>481</v>
+      </c>
+      <c r="V36" s="479">
+        <v>0</v>
+      </c>
       <c r="W36" s="53" t="s">
         <v>414</v>
       </c>
@@ -39462,7 +39521,7 @@
       <c r="B64" s="178" t="s">
         <v>466</v>
       </c>
-      <c r="C64" s="563" t="s">
+      <c r="C64" s="561" t="s">
         <v>467</v>
       </c>
       <c r="D64" s="171"/>
@@ -39506,11 +39565,11 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="558"/>
+      <c r="A65" s="556"/>
       <c r="B65" s="178" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="564"/>
+      <c r="C65" s="562"/>
       <c r="D65" s="171"/>
       <c r="E65" s="60"/>
       <c r="F65" s="151">
@@ -39956,8 +40015,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="515"/>
-      <c r="P79" s="529"/>
+      <c r="O79" s="534"/>
+      <c r="P79" s="536"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -39986,8 +40045,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="516"/>
-      <c r="P80" s="530"/>
+      <c r="O80" s="535"/>
+      <c r="P80" s="537"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -40016,8 +40075,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="515"/>
-      <c r="P81" s="529"/>
+      <c r="O81" s="534"/>
+      <c r="P81" s="536"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -40049,8 +40108,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="516"/>
-      <c r="P82" s="530"/>
+      <c r="O82" s="535"/>
+      <c r="P82" s="537"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -40208,8 +40267,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="531"/>
-      <c r="M87" s="532"/>
+      <c r="L87" s="538"/>
+      <c r="M87" s="539"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40241,8 +40300,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="531"/>
-      <c r="M88" s="532"/>
+      <c r="L88" s="538"/>
+      <c r="M88" s="539"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -40445,8 +40504,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="515"/>
-      <c r="P94" s="525"/>
+      <c r="O94" s="534"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -40478,8 +40537,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="516"/>
-      <c r="P95" s="526"/>
+      <c r="O95" s="535"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -45871,11 +45930,11 @@
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="527" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="527"/>
-      <c r="H259" s="528"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>491966.85000000003</v>
@@ -46449,12 +46508,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O79:O80"/>
@@ -46466,6 +46519,12 @@
     <mergeCell ref="H64:H65"/>
     <mergeCell ref="O64:O65"/>
     <mergeCell ref="P64:P65"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -46479,11 +46538,11 @@
   </sheetPr>
   <dimension ref="A1:X292"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="8" ySplit="3" topLeftCell="M52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M55" sqref="M55"/>
+      <selection pane="bottomRight" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -46512,18 +46571,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="533" t="s">
+      <c r="A1" s="509" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="533"/>
-      <c r="C1" s="533"/>
-      <c r="D1" s="533"/>
-      <c r="E1" s="533"/>
-      <c r="F1" s="533"/>
-      <c r="G1" s="533"/>
-      <c r="H1" s="533"/>
-      <c r="I1" s="533"/>
-      <c r="J1" s="533"/>
+      <c r="B1" s="509"/>
+      <c r="C1" s="509"/>
+      <c r="D1" s="509"/>
+      <c r="E1" s="509"/>
+      <c r="F1" s="509"/>
+      <c r="G1" s="509"/>
+      <c r="H1" s="509"/>
+      <c r="I1" s="509"/>
+      <c r="J1" s="509"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -46539,22 +46598,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="534" t="s">
+      <c r="W1" s="510" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="535"/>
+      <c r="X1" s="511"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="533"/>
-      <c r="B2" s="533"/>
-      <c r="C2" s="533"/>
-      <c r="D2" s="533"/>
-      <c r="E2" s="533"/>
-      <c r="F2" s="533"/>
-      <c r="G2" s="533"/>
-      <c r="H2" s="533"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="533"/>
+      <c r="A2" s="509"/>
+      <c r="B2" s="509"/>
+      <c r="C2" s="509"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="509"/>
+      <c r="F2" s="509"/>
+      <c r="G2" s="509"/>
+      <c r="H2" s="509"/>
+      <c r="I2" s="509"/>
+      <c r="J2" s="509"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -46608,10 +46667,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="536" t="s">
+      <c r="O3" s="512" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="537"/>
+      <c r="P3" s="513"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -50247,8 +50306,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="531"/>
-      <c r="M87" s="532"/>
+      <c r="L87" s="538"/>
+      <c r="M87" s="539"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50280,8 +50339,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="531"/>
-      <c r="M88" s="532"/>
+      <c r="L88" s="538"/>
+      <c r="M88" s="539"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -50484,8 +50543,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="515"/>
-      <c r="P94" s="525"/>
+      <c r="O94" s="534"/>
+      <c r="P94" s="530"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -50517,8 +50576,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="516"/>
-      <c r="P95" s="526"/>
+      <c r="O95" s="535"/>
+      <c r="P95" s="531"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -55910,11 +55969,11 @@
         <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="527" t="s">
+      <c r="F259" s="532" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="527"/>
-      <c r="H259" s="528"/>
+      <c r="G259" s="532"/>
+      <c r="H259" s="533"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>454344.37</v>

</xml_diff>